<commit_message>
added robustness formula, corrected to take interest rate into account
</commit_message>
<xml_diff>
--- a/results1.xlsx
+++ b/results1.xlsx
@@ -5,15 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeo\Desktop\master\S3\C++\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pigeo\Desktop\master\S3\C++\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9750" windowHeight="4980" xr2:uid="{C05CCDE3-ED8E-49DF-945E-43D0F56FFEC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9750" windowHeight="4980" activeTab="1" xr2:uid="{C05CCDE3-ED8E-49DF-945E-43D0F56FFEC8}"/>
   </bookViews>
   <sheets>
     <sheet name="flat rate 0" sheetId="1" r:id="rId1"/>
     <sheet name="with rates libor3m" sheetId="2" r:id="rId2"/>
+    <sheet name="flat rate 5% regular" sheetId="4" r:id="rId3"/>
+    <sheet name="flat rate 5% robustness" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Breakeven vol</t>
   </si>
@@ -34,6 +36,9 @@
   </si>
   <si>
     <t>Strike as % of initial spot</t>
+  </si>
+  <si>
+    <t>vol</t>
   </si>
 </sst>
 </file>
@@ -118,6 +123,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Breakeven vol, r = 0%</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -501,7 +531,1369 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Breakeven vol, libor3m file</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'with rates libor3m'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'with rates libor3m'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.50000222316089005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000111158044507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64999888841955489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70000222316089011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75000111158044502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84999888841955484</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90000222316089007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95000111158044498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4499988884195547</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.50000222316089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'with rates libor3m'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.34161999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30594900000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.272642</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.241314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.211669</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18349599999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15667600000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13126399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.10773099999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7684200000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4366199999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7914299999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.1894600000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.2415000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0145099999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-774E-410F-85B2-7052B20B9C5B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2015566672"/>
+        <c:axId val="2018166272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2015566672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2018166272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2018166272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2015566672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Breakeven vol, r = 5%</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'flat rate 5% regular'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'flat rate 5% regular'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.50000222316089005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000111158044507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64999888841955489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70000222316089011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75000111158044502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84999888841955484</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90000222316089007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95000111158044498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4499988884195547</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.50000222316089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'flat rate 5% regular'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2524099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.0713000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.40232E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.4443800000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.0312600000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E8F2-4819-8D01-1C5F26AB43AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1867457440"/>
+        <c:axId val="1865351776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1867457440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1865351776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1865351776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1867457440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>breakeven vol, r = 5%, robustness formula</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'flat rate 5% robustness'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vol</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'flat rate 5% robustness'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.50000222316089005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55000111158044507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64999888841955489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70000222316089011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75000111158044502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84999888841955484</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90000222316089007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95000111158044498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2499988884195548</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3000022231608901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3500011115804449</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4499988884195547</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.50000222316089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'flat rate 5% robustness'!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3437499999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2218700000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.66094E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.66094E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.8046900000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.9023399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6097399999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.8046900000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9023399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9511699999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.77897E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.2758099999999997E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBED-40FE-B0EF-A6A4DFD76962}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2015564592"/>
+        <c:axId val="1865369920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2015564592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1865369920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1865369920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2015564592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1057,6 +2449,1554 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1078,6 +4018,129 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{647A5BA2-1701-4C2D-84C9-07820AF931B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C76BFF-0F24-4046-8F36-67C652F0A3AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67648187-3059-4549-90E8-4BDF8D089763}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D572A3E5-DB52-46A4-91BF-EF081D3FC74A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1398,8 +4461,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1725,8 +4788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B23EA82-0D7B-4A4C-B59E-C1BCB2704A5A}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1747,7 +4810,7 @@
         <v>0.50000222316089005</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.34161999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1758,7 +4821,7 @@
         <v>0.55000111158044507</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.30594900000000003</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1768,8 +4831,8 @@
       <c r="B4" s="2">
         <v>0.6</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" s="3">
+        <v>0.272642</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1779,8 +4842,8 @@
       <c r="B5" s="2">
         <v>0.64999888841955489</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" s="3">
+        <v>0.241314</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1790,8 +4853,8 @@
       <c r="B6" s="2">
         <v>0.70000222316089011</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" s="3">
+        <v>0.211669</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1801,8 +4864,8 @@
       <c r="B7" s="2">
         <v>0.75000111158044502</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" s="3">
+        <v>0.18349599999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1812,8 +4875,8 @@
       <c r="B8" s="2">
         <v>0.79999999999999993</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" s="3">
+        <v>0.15667600000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1823,8 +4886,8 @@
       <c r="B9" s="2">
         <v>0.84999888841955484</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" s="3">
+        <v>0.13126399999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1834,8 +4897,8 @@
       <c r="B10" s="2">
         <v>0.90000222316089007</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" s="3">
+        <v>0.10773099999999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1845,8 +4908,8 @@
       <c r="B11" s="2">
         <v>0.95000111158044498</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" s="3">
+        <v>8.7684200000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1856,8 +4919,8 @@
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" s="3">
+        <v>7.4366199999999993E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1868,7 +4931,7 @@
         <v>1.0499988884195548</v>
       </c>
       <c r="C13" s="3">
-        <v>3.8422400000000002E-2</v>
+        <v>6.7914299999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1879,7 +4942,7 @@
         <v>1.1000022231608901</v>
       </c>
       <c r="C14" s="3">
-        <v>4.8264000000000001E-2</v>
+        <v>6.1894600000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1890,7 +4953,7 @@
         <v>1.1500011115804449</v>
       </c>
       <c r="C15" s="3">
-        <v>4.4397899999999997E-2</v>
+        <v>5.2415000000000003E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1901,7 +4964,7 @@
         <v>1.2</v>
       </c>
       <c r="C16" s="3">
-        <v>4.7309799999999999E-2</v>
+        <v>5.0145099999999998E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1923,7 +4986,7 @@
         <v>1.3000022231608901</v>
       </c>
       <c r="C18" s="3">
-        <v>3.2218700000000003E-2</v>
+        <v>6.3437499999999994E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1972,5 +5035,525 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3702DF3-AA8C-4CF2-8124-92552D325237}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1124.53</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.50000222316089005</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1236.98</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.55000111158044507</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1349.43</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1461.88</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.64999888841955489</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1574.34</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.70000222316089011</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1686.79</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.75000111158044502</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1799.24</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1911.69</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.84999888841955484</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2024.15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.90000222316089007</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2136.6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.95000111158044498</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2249.0500000000002</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2361.5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0499988884195548</v>
+      </c>
+      <c r="C13" s="3">
+        <v>6.2524099999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2473.96</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.1000022231608901</v>
+      </c>
+      <c r="C14" s="3">
+        <v>6.0713000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2586.41</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.1500011115804449</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5.40232E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2698.86</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5.4443800000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2811.31</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.2499988884195548</v>
+      </c>
+      <c r="C17" s="3">
+        <v>6.0312600000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2923.77</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.3000022231608901</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>3036.22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.3500011115804449</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3148.67</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3261.12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.4499988884195547</v>
+      </c>
+      <c r="C21" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3373.58</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.50000222316089</v>
+      </c>
+      <c r="C22" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09308C80-56E6-4A35-A036-2E7078BAF0C7}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1124.53</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.50000222316089005</v>
+      </c>
+      <c r="C2" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1236.98</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.55000111158044507</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1349.43</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1461.88</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.64999888841955489</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6.3437499999999994E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1574.34</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.70000222316089011</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1686.79</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.75000111158044502</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1799.24</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1911.69</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.84999888841955484</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2024.15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.90000222316089007</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2136.6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.95000111158044498</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2249.0500000000002</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3.2218700000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2361.5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0499988884195548</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.66094E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2473.96</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.1000022231608901</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1.66094E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2586.41</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.1500011115804449</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8.8046900000000004E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2698.86</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4.9023399999999998E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2811.31</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.2499988884195548</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.6097399999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2923.77</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.3000022231608901</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8.8046900000000004E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>3036.22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.3500011115804449</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4.9023399999999998E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3148.67</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2.9511699999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3261.12</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.4499988884195547</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.77897E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3373.58</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.50000222316089</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5.2758099999999997E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>